<commit_message>
chore(epic_app/admin.py): Changed admin pages to refer to import xlsx instead of csv.
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/keyagencyactionsquestions.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/keyagencyactionsquestions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardjoe\OneDrive - Stichting Deltares\Documents\04. Deltares Projecten\04.160. EPIC Response Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D413B0A-0247-4A22-B30E-99841F61E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B65A3F4D-8B9A-467B-9D5A-A26AAAEE8E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="5175" windowWidth="21600" windowHeight="10575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keyagencyactionsquestions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
   <si>
     <t>Program areas</t>
   </si>
@@ -40,6 +40,9 @@
     <t>Programs</t>
   </si>
   <si>
+    <t>Program description</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Question</t>
   </si>
   <si>
@@ -49,24 +52,43 @@
     <t>Water Resource Management</t>
   </si>
   <si>
+    <t xml:space="preserve">The dominant paradigm for WRM is “integrated water resources management (IWRM)”. While there is no official definition of IWRM, a commonly used definition is that it is “a process which promotes the coordinated development and management of water, land and related resources in order to maximize economic and social welfare in an equitable manner without compromising the sustainability of vital ecosystems and the environment” (GWP 2000). Recognized at the international level more than 30 years ago at the 1992 Earth Summit in Rio de Janeiro, Target 6.5 of Sustainable Development Goal 6 on Clean Water and Sanitation calls for the implementation of IWRM at all levels by 2030. 
+The basic objective of WRM is the management of water as a natural resource, the use of which is fundamental to all socioeconomic activities, but which at the same time plays a vital ecological function that needs to be protected. As such, WRM seeks to allocate water among different user sectors (such as water supply, agriculture, industry, and power generation) and water users. It promotes the development of water resources while also seeking to prevent or minimize water pollution and to ensure appropriate water quality. It sets and enforces minimum or environmental flows to enable people to meet basic needs and to protect aquatic ecosystems and the livelihoods of those who depend on those ecosystems. Many of the programs identified in the upper part of the EPIC Response Framework fall under the general, but not necessarily exclusive, domain of the WRM framework, including river basin planning, water resources infrastructure, and adaptable water allocation. It follows that an effective national framework for hydro-climatic risk management system generally requires a functional and comprehensive national framework for WRM. </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Is this an example question?</t>
   </si>
   <si>
     <t>Disaster Risk Management</t>
   </si>
   <si>
+    <t>DRM is a broad topic that has seen significant evolution over recent years, encapsulated by the recent Sendai Framework for Disaster Risk Reduction 2015-2030. Among the four priorities of the Sendai Framework is Priority 2: “Strengthening disaster risk governance to manage disaster risk”. This priority notes “the vital role of disaster risk governance at the national, regional and global levels in terms of the management of disaster risk reduction and ensuring the coherence of national and local frameworks of laws, regulations and public policies that, by defining roles and responsibilities, guide, encourage and incentivize the public and private sectors to take action and address disaster risk.”   
+Floods and droughts are invariably included among the types of natural hazards that are subject to a disaster risk management (DRM) framework along with storms, earthquakes, volcanoes, and disease outbreaks, as well as anthropogenic hazards such as transportation and industrial accidents. It follows  that, as with WRM, an effective national framework for hydro-climatic risk management includes the need for an effective, functional, and comprehensive national DRM framework.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> When did you add these examples?</t>
   </si>
   <si>
     <t>Drought Risk Management</t>
   </si>
   <si>
+    <t>Drought risk management is a complex endeavor that requires both WRM and DRM perspectives, but also necessitates going beyond these traditional domains. International recognition of the importance of droughts was reflected in the 1994 United Nations Convention to Combat Desertification (UNCCD) which calls upon decision makers and water and land managers to take a proactive, coordinated, and holistic approach to drought risk management.   
+The modern conception of WRM includes both “blue” and “green” water. Blue water is mainly water stored in rivers, reservoirs, lakes, and accessible groundwater aquifers, and is available for uses such as hydropower, water supply, and irrigation. Green water refers to the water that originates from precipitation, is stored in unsaturated soil, and is absorbed and undergoes transpiration by plants or is evaporated directly from the soil. Green water plays an irreplaceable role in global ecosystems and food production, accounting for around 80 percent of global food production and exclusively sustaining grassland and forest ecosystems (Liu and Yang 2010).  
+WRM policies, institutions, and infrastructure have, however, historically evolved to manage primarily blue water. Drought not only affects traditional blue water uses, but also has a profound impact on green water, particularly as regards agriculture and natural resources management. These domains thus must also be explicitly incorporated into drought risk management systems. Healthy land provides natural storage for fresh water. If it is degraded, it cannot perform that function. Managing land better and massively scaling up land rehabilitation are essential for building drought resilience and water security. Land restoration is the cheapest and often the most effective solution to improving water storage, mitigating impacts of drought, and addressing biodiversity loss. 
+DRM evolved primarily in response to immediate and devastating natural shocks such as earthquakes, storms, floods, and landslides. Drought, in contrast, is generally a slow-moving natural disaster in which the extent of the impact only emerges over time, sometimes years, and the understanding of future impacts are limited by the accuracy of weather and climate forecasts and socioeconomic drivers. Some of the elements of a DRM framework, such as efforts to mitigate hazards and the activation of emergency support systems, can also naturally be applied to drought risk management.
+In summary, although WRM and DRM are intimately linked to drought management, it is generally necessary to develop a specific drought framework that incorporates the unique elements of drought monitoring, impact assessment, and risk characterization, in addition to providing the basis for drought agricultural response and recovery programs. In some poorer countries with large rural populations, WRM and DRM frameworks may not even exist or may be underdeveloped, and in such cases the burden of managing droughts may fall primarily on the agriculture agency and local governments.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Can we add more examples?</t>
   </si>
   <si>
     <t>Flood Risk Management</t>
   </si>
   <si>
+    <t>In many countries, the combination of WRM, DRM, and Hrydro-Met sector frameworks—if properly synchronized—should address most issues related to flood risk management. However, some more advanced countries have also found it useful to adopt additional flood management specific laws or national policies to help bind these sector frameworks more closely together. Some examples are provided below:
+The European Union’s Water Framework Directive  and Floods Directive , between them require member states to adopt a common approach to river basin management and flood risk assessment and management planning. As shown in figure 3.4, in Japan there are three major interlocking laws related to flood risk management, the DRM Act, the River Act (which acts as a water resources law), and a specific Flood Protection Act. In the United States, the Federal Interagency Floodplain Management Task Force helps bring together all water-related agencies and was established under the 1975 Water Resources and Development Act</t>
+  </si>
+  <si>
     <t xml:space="preserve"> You will be adding more</t>
   </si>
   <si>
@@ -76,145 +98,309 @@
     <t>Local Government</t>
   </si>
   <si>
+    <t xml:space="preserve">Local governments play pivotal roles in responding to flood and drought disasters (World Bank 2019). As highlighted in Chapter 12, local governments need to work in concert with national DRM agencies to respond to floods. They serve as one of many channels to warn about floods, to help evacuate residents, to ensure public safety, to provide relief to impacted people, and to help guide recovery efforts. Chapter 11 notes how local governments can work in concert with national agencies on drought issues; they can help disseminate information as the drought unfolds, implement emergency drought measures, administer drought assistance, and support social protection programs.
+Local governments also play important roles in flood and drought risk mitigation (Gencer 2017). Chapter 10 on floodplain management highlights their central role in land use planning, building regulations, and preparing local flood mitigation plans. They also oversee urban water supply and drought contingency plans, as highlighted in Chapter 5. Local governments invest in localized water resources infrastructure to mitigate flood and drought hazards, including stormwater drainage systems, local flood control projects, and water supply and sanitation systems (typically through their water utilities). The capacity and authority of local governments to contribute to hydro-climatic risk management varies considerably among, and sometimes within, countries. A 2017 survey examined the authority, capacity, and responsibilities of 151 cities around the world with respect to disaster risk reduction. </t>
+  </si>
+  <si>
     <t>Public Participation &amp; Stakeholder Engagement</t>
   </si>
   <si>
+    <t>Agencies need to engage with the public and stakeholders to have effective programs for multiple reasons. First, the information that stakeholders bring to the program design is crucial to ensuring its success. Second, any program ultimately seeks to influence the decisions and actions of the impacted public and thus their understanding and acceptance is necessary. Third, public monitoring and participation generate incentives and pressure for the agency to continuously improve the program.
+Ideally, public participation operationalizes a two-way communication avenue between agencies implementing programs and the communities they serve where both can inform, learn, and benefit from the process. The International Association for Public Participation (IAP2) has developed core principles that should be internalized by all agencies and incorporated into each program highlighted in this report. 
+While there are numerous advantages associated with public participation and stakeholder engagement, if not properly structured and targeted it may not be fully successful and can even be counterproductive. For example, a substandard public participation process can amplify privileged voices and underrepresent marginalized groups, resulting in so-called elite capture. To implement effective public participation and stakeholder engagement, agencies must make it a priority, generate a robust knowledge base of the circumstances and conflicting interests of the communities they serve, build capacity and train staff, develop targeted and inclusive participatory processes, and allocate the necessary time and budget.</t>
+  </si>
+  <si>
     <t>Social Inclusion</t>
   </si>
   <si>
+    <t>In every country, certain groups face barriers that prevent them from fully participating in the nation’s political, economic, and social life. These groups may, to varying degrees, be excluded from political processes, economic opportunities, and government services. Social inclusion has been defined as the process of improving the terms on which individuals and groups take part in society—improving the ability, opportunity, and dignity of disadvantaged people (World Bank 2020). Individuals or groups can be marginalized in terms of their socioeconomic status, age, gender, sexual orientation, race, ethnicity, religion, disability, or citizenship status, among other factors. Marginalized individuals and groups can be found in all countries across the development spectrum. 
+Social inclusion matters in and of itself, emanating from the principles of human rights and social justice. It also matters because social exclusion can carry substantial social, political, and economic costs. Exclusion often has a negative impact on human capital, preventing individuals from achieving their full potential at multiple levels, resulting in lowered education levels and impaired health. There is ample evidence that human capital is closely correlated with economic development (World Bank 2013). Moreover, excluding large groups of people can destabilize society, generating political unrest or civil strife.</t>
+  </si>
+  <si>
     <t>Education &amp; Risk Communication</t>
   </si>
   <si>
+    <t xml:space="preserve">Each agency should strive to help educate the general public and promote professional development. Educational programs increase public awareness and knowledge about sector issues. In doing so, they provide the public and professionals with the necessary evidence to make informed decisions and to take responsible action. Since education has strong public good characteristics, the agency should use part of its budget and professional expertise for educational programs. These can be delivered directly by the agency or in partnership with professional organizations, universities, schools, civil society, and businesses. The agency can provide grants or technical assistance to its partner organizations to further support educational activities. Risk communication is often distinguished from emergency or crisis communication. Risk communication needs to be done before a hazardous event occurs to inform the public about their potential exposure and to encourage them to engage in precautionary measures to avoid, reduce, and transfer these risks. Emergency communication is then used to inform people once the event is imminent or underway. After the emergency or crisis, risk communication comes into play again to help present what occurred on the basis of lessons learned (OECD 2016a). Communicating hydro-climatic risk, especially in the context of a changing climate, is challenging. Estimating risks embodies many complex concepts, including at its core the probabilistic assessment of different hazard levels—which is typically beyond the level of most non-experts to fully grasp and act upon. Research on risk communication has shown that risk is best understood when the communication is simple, tangible, relevant, and personal.  Risk should be communicated in a way that is not only clear and quantifiable, but also that leads people to recognize how they could be personally affected and that motivates them to act. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Scientific Collaboration </t>
   </si>
   <si>
+    <t>The scientific complexity of hydro-climatic risk management is enormous. The expertise to address this complexity, for both social and natural sciences, spans a broad range of organizations, including national agencies, research institutes, international organizations, and the private sector. The traditional model of a “supplier” of scientific information—such as a research institute, and a “user” of the information—such as a national agency, is outdated. There is a growing recognition of the need to have both science-informed policy and policy-informed science to deal with climate adaptation (Daniels and others 2020). In other words, scientific organizations and national agencies need to effectively collaborate to generate effective science applied to flood and drought risk management. Collaboration between national agencies and the research community to generate science-informed policy and policy-informed science is not an easy task. A recent framework proposed by the Stockholm Environment Institute provides some general guidelines. Key elements include: (1) improving the way participants work together by designing co-exploration and co-production processes that bring together different fields across the science-society interface; (2) working together to understand or define decision-relevant needs of the agency; and (3) increasing the capacity for collaboration by building strong networks (Daniels and others 2020).</t>
+  </si>
+  <si>
     <t>Open Data</t>
   </si>
   <si>
+    <t>We are living in the “Information Age” where the access and control of information is the defining characteristic of our time. This Age fosters disruptive technologies and new ways of doing business that can both be chaotic and transforming. The national agencies involved in hydro-climatic risk management, including WRM, DRM, Hydro-met, agriculture, and natural resources management agencies, produce large amounts of information. This information can take various forms, such as on-ground and space-based monitoring data, GIS-based maps, model codes, and reports. Making this information freely available to other agencies and the public can turbocharge advances in flood and drought management through three pathways: 
+First, since the different programs in the Framework are interrelated, sharing information will allow agencies to do their work better and collaborate more productively in a joined-up manner. As an example, information on watershed health collected by the natural resources agency serves as a critical input to river basin planning exercises led by the WRM agency. These types of linkages exist throughout all programs highlighted in this report.
+Second, open data produces a better-informed public that can engage more effectively with national agencies, resulting in more effective programs. Since information is power, open data can be used to hold national governments and their agencies more accountable and increase transparency. Open data can also help different groups make better informed risk management decisions, ideally complemented with education and risk communication programs.
+Finally, open data can help drive innovation, economic growth, and environmental sustainability. As highlighted in the section on scientific collaboration, much of the expertise for managing flood and drought risks and adapting to a changing climate exists outside of national agencies. Providing these scientific and research organizations with information will enable them to undertake more accurate studies and propose better solutions. As a corollary, publicly-funded research should also be brought into the public domain, and some private companies may also find it beneficial to publicly share information. Open data will also help the private sector to develop products that can help to reduce hydro-climatic risks. As an example, the insurance industry needs extensive information—much of it collected by government—to formulate and properly price flood or drought insurance.</t>
+  </si>
+  <si>
     <t>Hydrological and Meteorological Services</t>
   </si>
   <si>
     <t>National Framework for NMS/NHS Services</t>
   </si>
   <si>
+    <t>Meteorological services are often governed by a national meteorological law. If there is a combined NMS/NHS, then the law also includes hydrological topics. In other cases, hydrological issues are typically addressed through the water resources law. In cases where there are separate meteorological and hydrological laws, it is extremely important to make sure that these two legal and regulatory regimes are seamlessly integrated.
+The basic legal and regulatory framework for hydro-met services has been described in detail in a 2013 World Bank report entitled “Weather and Climate Resilience” (Rogers and Tsirkunov 2013). Some of the key topics to be addressed include defining a clear mandate, including all relevant actors beyond the NMS/NHS, open data principles, revenue generation, research and development, and authorization to arrange for joint monitoring and forecasting of meteorological and hydrological disasters among government agencies. 
+Hydromet laws need to evolve quickly to adjust to changing technology and to meet the increasing demands from users, specifically from the WRM, DRM, and Drought Communities. Often there is an overemphasis on NMS/NHS functions with insufficient attention paid to the broader need of providing weather and hydrological services. This can result in obligations and regulations imposed on others and insufficient accountability for what the NMS/NHS should produce.</t>
+  </si>
+  <si>
     <t>National Water Data Program</t>
   </si>
   <si>
+    <t xml:space="preserve">The collection of hydrological data is often spread out across multiple national agencies that collect different types of information, for example surface water, groundwater, and water quality. Ideally, there would be a single (or potentially multiple) program to consolidate this information and make it freely and easily accessible to the public. There are various approaches for doing this, including creation of hydro-informatics centers, open water data initiatives, and the establishment of national water data systems. Ideally the NHS or natural resources management agency should be mandated to facilitate a national water data program and enter into interagency agreements and operational protocols to ensure the smooth flow of high-quality data. This would generate enormous value added for water-related planning, design of water infrastructure, and research. Every agency working on hydro-climatic risk management would benefit from combining their water-related information through a national water data program. </t>
+  </si>
+  <si>
     <t>Drought Monitoring and Impact Assessment</t>
   </si>
   <si>
+    <t>This topic is explored in depth in Chapter 11, which notes that droughts generally evolve gradually over time, cover large areas, and have broad social, economic, and environmental impacts. A national drought monitoring program is usually the best approach, requiring a nexus of cooperation among NMS/NHS, WRM, agriculture, and DRM agencies. The NMS/NHS plays a critical role in monitoring drought hazards by providing analysis on “dryness” conditions (World Bank 2019). However, this hydro-met information is only part of the story, as droughts are assessed primarily by their impacts on farmers, cities, and the environment. The NMS/NHS needs to work closely with the other agencies, local governments, and other parties to better understand vulnerabilities, risks, and appropriate drought response actions. The National Drought Framework discussed in Chapter 3 should help facilitate interagency agreements and operational protocols to ensure this nexus operates smoothly.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Flood Forecasting and Warning </t>
   </si>
   <si>
+    <t xml:space="preserve">This topic is explored in depth in Chapter 12, which notes that different types of flood require different approaches. Flood forecasts and warning require a cooperation nexus among the NMS/NHS, WRM, and DRM agencies. Clear interagency agreements and operational protocols need to be developed to ensure that this nexus operates efficiently. One option is to establish a National Flood Center which can foster collaboration and flexibility to handle a variety of floods. </t>
+  </si>
+  <si>
     <t>Agrometeorological Advisory Services</t>
   </si>
   <si>
+    <t>Agro-Climate Advisory Services: As highlighted in Chapter 11, farmers are particularly prone to be affected by fluctuations in weather and by extreme hydro-climatic events, particularly droughts. It is estimated that 20-80 percent of the inter-annual variability of crop yields is associated with weather phenomena, and 5-10 percent of national agricultural production losses are associated with climate variability (WMO 2019). NMS/NHS can team with agriculture agencies to help farmers better cope with climate variability and extreme events through the provision of agro-climate advisory services. Farmers receive information at different time scales to help them make informed decisions. For example, weather forecasts up to a week in advance can help them make decisions regarding planting and harvesting, fertilizer application, and irrigation requirements. Seasonal forecasts on the order of months can inform cropping decisions and livestock strategies.</t>
+  </si>
+  <si>
     <t xml:space="preserve">National Climate Assessment </t>
   </si>
   <si>
+    <t xml:space="preserve">An NCA helps to inform the country about already observed changes, the current status of the climate, and anticipated trends for the future.  It typically provides analysis of the effects of climate change on the environment, agriculture, health, water resources, and coastal areas, and includes an analysis of flood and drought risks. An NCA can help guide adaptation actions across society by informing planning at all levels, influencing private investment decisions, and spurring actions to enhance climate resilience. The development of an NCA needs to be a collaborative effort with many national agencies, as well as other stakeholders. Although lead responsibility for the formulation of an NCA will vary by country, in every case the NMS/NHS needs to be front-and-center in the process as the leading authority on climate. 
+An NCA is a complex undertaking and less-affluent countries may need international assistance. Global experience has shown that the process of formulating an NCA and pondering the manifold impacts of climate change and its attendant risks is as important as the actual report—which in any case needs to be periodically updated. The various national agencies can build upon the knowledge gained through the NCA to develop more climate-sensitive sector strategies. </t>
+  </si>
+  <si>
     <t>Flood and Drought Risk Mitigation and Contingency Planning</t>
   </si>
   <si>
     <t>Integrated River Basin Planning</t>
   </si>
   <si>
-    <t>Do you have the system(s) in place to foster correct institutional arrangements?</t>
+    <t xml:space="preserve">River basin plans guide the development, management, allocation, and use of water and related resources within a specific geographical area. Ideally, this is an actual river basin, but in some cases the planning area may be limited due to transboundary constraints or in order to ensure a more tractable planning size. In some countries, a single river basin is simply too large to plan as a single unit, so it is necessary to divide it into sub-basins. River basin plans are typically integrated plans, addressing water quantity, water quality, surface water and groundwater, and the protection of water and aquatic ecosystems while enabling the integration of upstream and downstream interests. Basin plans should also include issues such as institutional responsibilities, implementation arrangements, budgets, and monitoring. </t>
   </si>
   <si>
     <t>Coastal Zone Management Planning</t>
   </si>
   <si>
+    <t xml:space="preserve">More than 600 million people, around 10 percent of the global population, live in coastal areas that are less than 10 meters above sea level (UN 2017). These areas are particularly vulnerable to flooding from storms and the associated storm surges that drive seawater onto coastal flood plains. Coastal zones can also be vulnerable to water shortages and droughts with the additional risk of saline intrusion (and therefore contaminated groundwater) as a result of groundwater over-abstraction. Climate change also directly impacts coastal communities due to rising sea levels and increasing storm frequencies and magnitudes in many areas. 
+The most comprehensive paradigm for coastal zone management is Integrated Coastal Zone Management (ICZM), a multi-sectoral, stakeholder-informed coastal zone equivalent of river basin planning, which seeks to promote economic development in the coastal zone while also protecting valuable coastal ecosystems. These ecosystems are often important for tourism and fisheries, and act as coastal barriers against storm surges. Unlike river basin planning, ICZM has not been fully mainstreamed into most countries’ planning processes, probably reflecting the complexity of the exercise. 
+Particularly in countries or coastal areas with extensive deltas, coastal zone planning must of necessity be linked to river basin management planning. That is because the delta represents the terminus of a river basin, where freshwater flows mix with seawater and bring sediments, nutrients, and pollutants that have a profound impact on coastal ecosystems. ICZM is also fundamentally intertwined with marine spatial planning by virtue of common geomorphological dynamics and the ecosystems providing services (such as flood protection) and goods to coastal economies.
+Coastal zone management plans provide the overall framework for flood management programs operating in coastal areas and should help inform local flood management plans for jurisdictions located along the coastline. They also help in establishing priorities for investments related to coastal barrier management, including protection and restoration activities, and the prioritization of areas where “hard” coastal defenses such as sea dikes or flood walls may be necessary. </t>
+  </si>
+  <si>
     <t>Urban Water Supply Planning</t>
   </si>
   <si>
+    <t>Urban water supply and sanitation utilities (hereafter “water utilities”) typically prepare master plans to define system-wide strategies and guide capital improvement projects to cope with population growth, regulatory requirements, and infrastructure renewal needs. In order to ensure that current, medium- and long-term water needs can be met, such master plans usually also include what are described in this report as an Urban Water Supply Plan (UWSP) that helps to mitigate drought risks by identifying potential supply-side and demand-side options. Potential supply-side options may include the construction of infrastructure in the form of new reservoirs, long-distance conveyance structures, water reclamation and desalination plants, development of new groundwater wellfields, and the purchase of water from bulk suppliers. Potential demand-side options may include reducing physical losses, promoting water conservation, and adjusting water pricing. Water quality may also be factored into a water supply plan, as poor raw water quality can potentially reduce the availability of potable water.</t>
+  </si>
+  <si>
     <t>Irrigation Water Supply Planning</t>
   </si>
   <si>
+    <t>Irrigation service providers are usually the largest users of water in a river basin and are accordingly also key stakeholders in river basin management planning. The notion of the irrigation service provider encompasses a range of different actors depending on the national context and may include an irrigation department in a ministry (such as the agriculture ministry or even the WRM ministry), a separate irrigation ministry, a semi-autonomous national or regional public irrigation agency, or farmer-managed water user organizations (variously described as “irrigation districts”, “water communities”, or “water user associations”), which may have their own direct access to water sources or which may in turn be supplied in bulk by public irrigation service providers. 
+Because of the volumes of water involved, irrigation service providers are generally required to demonstrate more flexibility in their water allocations than are other uses such as water utilities or hydropower operators, and thus play a critical role in basin drought contingency plans. At the same time, though, reduced irrigation water availability may reduce crop production (and therefore influence food prices and food security) and adversely affect rural livelihoods. 
+In order to ensure sustainable and long-term operation, best practice suggests that irrigation service providers should periodically prepare irrigation scheme master plans that cover all aspects of their service, including asset management and capital planning. Ideally too, and depending on the socioeconomic context, an irrigation service provider should prepare an Irrigation Water Supply Plan (IWSP) that looks at long-term resource planning to ensure that adequate water is available to meet farmers’ existing and future uses, particularly considering changing cropping patterns and climate change. This involves balancing water supply and demand alternatives, while also considering water quality, to ensure long-term sustainability. 
+There are typically several critical elements in an IWSP. It should include seasonal and monthly water budgets based on quantifying all inflow and outflow components for the service area, such as: crop water use, non-beneficial evaporation, groundwater seepage, and return flows. The IWSP should present water management objectives based on the water budget as a guide to improve system efficiency or meet other objectives. This should include a program of actions to help meet these objectives, including various water conservation approaches. In many schemes there is a need to first improve flow measurement and water control within the canal network through a modernization program. 
+It is also important to ensure that irrigation service providers prepare a Drought Plan describing actions for drought preparedness as well as allocations of water supply during drought conditions. Unlike urban WSCPs, the IWSP Drought Plan may not need to be a stand-alone document as irrigation service providers generally have more flexibility during drought periods than urban water utilities which are required to maintain minimum service levels to protect public health.</t>
+  </si>
+  <si>
     <t>Local Flood Risk Mitigation Planning</t>
   </si>
   <si>
+    <t>Missing</t>
+  </si>
+  <si>
     <t>Healthy Watersheds</t>
   </si>
   <si>
     <t>Agriculture Policies and Climate Smart Agriculture</t>
   </si>
   <si>
+    <t>Agricultural Economic Policies:  Agricultural economic policies can have a significant impact on land use, sometimes motivating farmers to grow inappropriate crops and utilize excessive amounts of water. To ensure food security and in conjunction with the Green Revolution starting in the 1960s, many governments adopted subsidy programs to promote the production of key staple crops (such as rice, wheat, and maize), support poor farmers, and keep food prices low. This helped to both combat rural poverty and ensure food security. These subsidies took the forms of below-cost irrigation water, subsidized inputs such as fertilizers and pesticides, and crop price support programs. Although in many countries these policies did in fact increase the supply of cheap food and address food security concerns, they also contributed to land degradation and water use inefficiency (Pingali 2012).
+Adjusting these agricultural policies to ensure the availability of nutritious food for the poor while reducing the environmental impacts of agriculture is the paramount agriculture policy imperative for the 21st century. It will not be politically easy, as many vested interests have emerged around existing subsidy regimes and governments are understandably wary about tampering with policies that may affect the production of food staples. Yet a Green Revolution 2.0 (GR2.0) is needed—and is emerging—to meet the world’s food demands, ensure environmental sustainability, and meet the challenges of climate change. 
+By 2050, the global population is projected to increase by about one-third, which will require a 70 percent increase in food production. GR 2.0 needs to not only increase basic cereal productivity (for example, wheat, rice, and corn) to meet the demand for staples, but also to make more land available for higher value and more nutritious crops, such as fruits, vegetables, and legumes. In addition, it should allow for the movement of labor out of agriculture when other economic opportunities provide greater returns. GR 2.0 must also improve the tolerance of crops to stresses, both climatic and biotic (pest and disease). Improved varieties that are tolerant to drought or excess water would enhance smallholder productivity in marginal environments and provide tools to adapt to climate change (Pingali 2012).
+Agriculture agencies, working in collaboration with farmers and agribusiness, need to show leadership in this transition to a GR 2.0. They can adjust agricultural policies to focus on improving productivity, gradually reducing subsidies that distort incentives for sustainable land management, and fund programs that support climate-smart agriculture. Governments can also work with the private sector and farmers to promote the use of new technologies, such as a greater focus on precision agriculture, the internet of things (IoT) and the use of big data—sometimes referred to as “agriculture 4.0” (De Clercq and others 2018). 
+Climate-Smart Agriculture Programs: Agricultural water and soil conservation programs have historically been a focus area for mitigating drought hazards. As an example, the U.S. Soil Conservation Service was created in response to the great Dust Bowl in the American prairies in the 1930s. In response to climate change, the approach has been broadened to include climate-smart agriculture (CSA). CSA aims to improve agricultural and livestock productivity while delivering greater resilience to climate change and lowering greenhouse gas emissions.</t>
+  </si>
+  <si>
     <t>Forest Management</t>
   </si>
   <si>
+    <t xml:space="preserve">The natural resources agency has several different options for managing forests on public lands depending on the specific context. Although this is a vast and complex topic, table 7.2 below presents four general management approaches for illustrative purposes.  These approaches are not mutually exclusive. For example, within the same forest areas, the natural resources agency may reserve some land for conservation, ensure sustainable forestry in public and private lands, and enter into arrangements with local communities including indigenous groups. </t>
+  </si>
+  <si>
     <t>Wetlands Management</t>
   </si>
   <si>
+    <t>There are a variety of approaches to wetlands management which are summarized below in table 7.4. As with forest management, these approaches are not mutually exclusive. National wetlands management programs might be linked to global efforts, particularly the Ramsar Convention, which currently has 171 Contracting Parties. The Ramsar Convention’s mission is “the conservation and wise use of all wetlands through local and national actions and international cooperation, as a contribution towards achieving sustainable development throughout the world.” National programs might benefit from the resources and analytical work provided with the Ramsar bodies (in particular from the Scientific and Technical Review Panel). They also can contribute to global monitoring efforts such as the Global Wetland Outlook.</t>
+  </si>
+  <si>
     <t>Local Watershed Management Organizations</t>
   </si>
   <si>
+    <t xml:space="preserve">These organizations can help provide a critical link between national agencies and local communities. This linkage is important because national agencies may have substantial financial resources and technical expertise, but communities often have a better sense of local priorities and are responsible for undertaking many of the actions supported by various natural resources management and agricultural programs. 
+In practice, WaMOs can follow hydrological or political boundaries and take on a variety of different forms and geographical coverage. In some cases, they may be legally constituted organizations that operate independently of the government. In other cases, the local government may have a specialized unit that helps organize and represent the community in its interactions with national agencies. An important consideration is that a WaMO needs to be able to take a broad landscape perspective within its area of jurisdiction and to understand how that area is nested into a larger watershed perspective. Agriculture and natural resources agencies should support and nurture WaMOs for a variety of reasons. WaMOs serve as an ideal conduit for public outreach and communication programs. WaMOs can also serve as a channel for implementing programs, either through block grants to WaMOs or helping to link potential beneficiaries with specific agency programs. WaMOs can also help national agencies better address social inclusion issues by providing linkages with marginalized groups such as indigenous groups, women, and landless populations. National agency support for WaMOs can take many forms, including helping in their legal establishment, funding, and providing technical assistance and training. </t>
+  </si>
+  <si>
     <t>Watershed Planning</t>
   </si>
   <si>
+    <t>Local WaMOs working in partnership with natural resources and agriculture agencies can help address issues on a relatively small scale. It is important also to have a periodic (for example every five years) planning or assessment exercise that looks at the entire watershed and identifies key problems, objectives, and high priority activities. A watershed management plan provides an opportunity for the agriculture, natural resources, and WRM agencies to examine the effectiveness of their various programs to promote healthy watersheds and adjust where necessary. It also gives local WaMOs an opportunity to better understand how their jurisdictions are affected by and contribute to larger watershed dynamics. 
+Information from watershed monitoring is an important input for watershed management plans. This should be focused on aspects such as the ecological conditions and trends of key natural assets (such as strategic wetlands, forests, soil erosion, water quality and quantity, and floods and droughts), helping establish cause-and-effect relationships between natural assets and ecosystem services, and informing and updating the implementation and effectiveness of specialized programs. A strong and continuous watershed monitoring program can provide a structured framework for adaptive watershed management by associating indicator thresholds with management activities (Shames and others 2017). 
+Watershed planning should be done in a collaborative process with all relevant agencies, and in a participatory manner with a wide range of stakeholders including the local WaMOs. The watershed management plan should feed into the river basin plan and vice versa. This collaborative arrangement between the various agencies is a classic example of the type of joined-up government approach required to address hydro-climatic risk management.</t>
+  </si>
+  <si>
     <t>Water Resources Infrastructure</t>
   </si>
   <si>
     <t>Water Resources Investment Policy</t>
   </si>
   <si>
+    <t>There is a clear need to increase funding for upgrading and constructing new water resources infrastructure, particularly to address the increasing hazards associated with climate change (HLPW 2018). WRI generates a mix of public and private benefits, yet it is generally funded by the government. Since public budgets are constrained, policies should be adopted which promote the efficient use of these funds. Investment efficiency is also important from an equity perspective because in many cases the costs (in terms of high levels of public subsidies) for WRI are borne by all taxpayers while the benefits go only to a much smaller group. Finally, national WRM agencies that depend entirely on a general budget and operate in a non-commercial manner may potentially be driven by political motivations, rent seeking, or local elite capture that distorts the decision-making process (Molle 2008).
+Ideally, WRI investment decisions should be guided by sophisticated economic and environmental analysis to determine whether a proposal is justified from a broad economic perspective; this also helps to ensure a reasonable project size and cost. An economic analysis is used to determine whether a proposed project will be a worthwhile investment. It would account for all benefits and costs regardless of who is affected. An economic analysis allows for fair comparisons to be made between alternatives and demonstrates why a proposed project can be considered the best solution to meet the overall objectives. More sophisticated economic analysis can consider environmental and social costs and benefits and thus provides a useful tool, along with the technical, financial, environmental, and social assessments, to appraise a project. It is particularly important to consider the co-benefits of associated green infrastructure when analyzing a project proposal (Browder and others 2019). Ideally, economic analysis should be integrated into a broader environmental and social impact assessment (ESIA) that can be used as the government’s primary decision-making document. 
+Although WRI is typically financed by the government, there are opportunities to recover some costs by charging water users, for example by selling bulk water supply to water utilities and irrigation schemes or by generating power from multi-purpose dams. Methods for allocating costs for multi-purpose reservoirs and water conveyance systems have been developed, allowing for more equitable cost recovery policies from water users (OCDE 2017).
+In many cases, the national government will help fund local flood control projects or the development of new water sources such as reservoirs or groundwater well fields. When funds are offered on a 100 percent grant basis there is a tendency for local governments to overbuild and undermaintain the WRI. Thus, adopting reasonable cost-sharing policies will encourage local governments to make better economic decisions, since the use of their scarce funds is also at stake. Attaching conditions to national funding of local WRI can also be used to incentivize local governments to adopt better and lower-cost management practices, for example by promoting the use of non-structural approaches for flood management or water conservation.</t>
+  </si>
+  <si>
     <t>Dam Safety</t>
   </si>
   <si>
+    <t xml:space="preserve">Dams comprise critical infrastructure to meet increasing demands for water, food, energy, and flood control. The failure of a dam can potentially have catastrophic impacts in terms of downstream flooding, as well as by removing an asset that communities are reliant upon to reduce flood hazards and to supply water. The two most common causes of dam failure are “overtopping” of earth dams, and foundation problems that are sometimes triggered by earthquakes. The proximate causes of dam failures, however, are often complex and myriad, and could include factors such as inappropriate design standards, bad siting decisions, poor construction, inadequate monitoring and maintenance, poor operational decisions, and lack of emergency planning. Dam safety programs are intended to address these shortcomings by ensuring a comprehensive life cycle approach.
+Dams are typically owned and operated by a wide variety of organizations. WRM agencies may themselves operate dams for multi-purpose use such as flood control, water supply, hydropower, and recreation. Energy agencies or companies may operate dams primarily for hydropower but may also include other uses. Agriculture agencies, and individual irrigation surface providers, often rely upon dams to provide water supply for irrigation systems. Water utilities often own and operate their own reservoirs to meet their water supply needs. Many of these dams are typically either constructed from soil or concrete, with a wide variation in dam and associated reservoir size. Ensuring that all these dams are regulated under an appropriate national dam safety management program is an indispensable element of hydro-climatic risk management.
+The core principle of dam safety management is the notion of shared responsibility. The owner is responsible for ensuring the safety of a dam, for operating and maintaining it in a safe condition, and for ultimately assuming criminal and civil liability in the event of a failure. The dam safety regulator is responsible for protecting the safety of the public by establishing dam safety standards and ensuring that these are fully implemented. </t>
+  </si>
+  <si>
     <t>Flood Infrastructure Safety</t>
   </si>
   <si>
+    <t xml:space="preserve">River and coastal flood control infrastructure provide many of the same functions as dams—essentially holding water back—and faces many of the same risks. Flood control embankments can include levees that protect land that is normally dry but that may be occasionally flooded, and dikes that protect land that would naturally be underwater most of the time. Tidal gates are important for coastal flood control and can help protect against storm surges. Large pump stations that help evacuate flood waters are critical elements of many flood control systems.
+Flood embankments are typically constructed from soil and are sometimes armored with concrete. They are prone to collapse when overtopped and they can suffer foundation failures like dams do. Flood walls are constructed from concrete, and in some cases steel, and may also fail from overtopping or foundation failures. Flood embankments may also be integrated into transport infrastructure, with roads or railway lines situated on top of the embankments. In some cases, specific sections of flood embankments may be designed to be easily breached (these are called fuse plugs). When flood levels in a river are dangerously high, the fuse plugs allow water to be channeled into areas that pose the lowest risk, such as agricultural areas with minimal numbers of structures. Although a flood control infrastructure failure is generally not as immediately catastrophic as a dam failure, it can have a significant impact over a large geographical region as river or coastal flood waters pour into low-lying areas. As an example, the devastating floods in New Orleans during Hurricane Katrina in 2005 were caused primarily by the failure of levees (ASCE 2017).
+Like dams, flood control infrastructure is often owned or operated by multiple entities. Larger infrastructure is typically constructed by the WRM agency, which may keep control of operations or maintenance or turn them over to local governments. In some cases, local governments or private industries, such as industrial estates, may construct their own flood control infrastructure. However, a basic challenge for flood safety can be identifying precisely who owns the infrastructure or sections of flood embankments and who is therefore responsible for maintaining them and ensuring their integrity. This is because many flood embankments have been built up and extended over decades or even over centuries. Consequently, few were originally designed or constructed to modern standards. In addition, records of their construction and historical performance may not exist. Moreover, they may stand for much of their lives without being loaded to design capacity, which can create a false sense of security in the level of protection they will provide.
+Flood infrastructure is typically composed of long linear structures that are only as strong as their weakest links. The structures can suffer from several potential deficiencies, such as old age, poor construction, and inadequate maintenance. They can also experience damage from burrowing animals and human activity, such as illegal construction on or adjacent to flood control infrastructures, illegal sand exploitation and storage of building materials, and overloaded vehicles travelling on embankments. They also are typically subject to encroachments by third-party objects that are constructed or installed over, under, or through the structures. Those encroachments can adversely affect flood control infrastructure integrity, but are not always fully recorded or documented. </t>
+  </si>
+  <si>
     <t>Water Allocation and Groundwater Management</t>
   </si>
   <si>
     <t>Flexible Water Allocation</t>
   </si>
   <si>
+    <t>WRM agencies should manage water allocations to ensure that water is not overallocated and that there is enough slack in the system to help mitigate drought impacts. This includes having a formal system of adaptable water allocations whereby water can be transferred from lower value users to higher value users, for example through administrative decisions, negotiated settlements, or water markets.</t>
+  </si>
+  <si>
     <t>Conjunctive Groundwater Management</t>
   </si>
   <si>
+    <t>This program involves balancing surface water and groundwater use, including managed groundwater recharge where possible, and ensuring that groundwater is available as a strategic reserve to help meet demand during droughts. Where groundwater aquifers exist, they provide an ideal water storage option. Too often, however, aquifers are overexploited resulting in unsustainable yields thus diminishing their effectiveness as strategic sources of water during droughts.</t>
+  </si>
+  <si>
     <t>Floodplain Management</t>
   </si>
   <si>
     <t>Floodplain Mapping</t>
   </si>
   <si>
+    <t>To properly manage river and coastal floodplains, the hazards should be well understood and communicated to local governments and the public. This is an enormously complex and continuous process that the DRM or WRM agency typically manages due to the technical challenges involved. It cannot be done quickly and needs to be constantly updated as flood hazards change over time due to climate change, watershed development, and new water resources infrastructure.</t>
+  </si>
+  <si>
     <t>Floodplain Regulation</t>
   </si>
   <si>
+    <t xml:space="preserve">Floodplain regulation helps to reduce exposure and vulnerability of people and assets and has two dimensions: (1) a permitting process to authorize development and activities; and (2) standards and codes to reduce the vulnerability of buildings and facilities. Land use management is generally a local government responsibility, and local governments should have their own specific floodplain management units. Some countries have even created multi-jurisdictional floodplain authorities to manage entire river or coastal stretches. The DRM agency has an important role to play in helping local governments by defining permitting guidelines and developing uniform standards. In some cases, the DRM agency may be legally mandated to oversee the implementation of local government floodplain regulations. </t>
+  </si>
+  <si>
     <t>Local Flood Mitigation Planning</t>
   </si>
   <si>
+    <t>River basin and coastal management planning are the tools generally used to reduce overall flood hazards at the regional level with a focus on watershed health and large-scale water resources infrastructure. Local flood mitigation planning plays an important complementary role to basin planning, and may often be part of a broader multi-hazard local government mitigation plan that includes other potential threats, such as earthquakes, landslides, and fires. Local flood mitigation plans go beyond regulation to proactively manage risks by identifying priority actions, such as refining land use plans and regulations, identifying infrastructure projects, conserving and restoring natural systems, and implementing educational and awareness programs. The DRM agency has an important role in providing guidelines and technical assistance to local governments in the formulation of flood mitigation plans. In some cases, the DRM agency may be legally mandated to oversee local government flood mitigation plans.</t>
+  </si>
+  <si>
     <t>Drought Monitoring</t>
   </si>
   <si>
     <t xml:space="preserve"> Drought Monitoring Program</t>
   </si>
   <si>
+    <t xml:space="preserve">A comprehensive Drought Monitoring Program (DMP) encompasses two interrelated activities: (1) the monitoring and forecasting of meteorological and hydrological conditions; and (2) the assessment of actual and potential on-the-ground drought impacts and risks. The DMP should classify and report on the level of drought for specific regions of the country. The designations often range from 1 to 5, from a low level (1) of “abnormally dry” to the highest level (5) of “an exceptional drought”. The designation of a drought level is important because it should help communicate the relative severity of the drought to different parts of the country and trigger actions identified in the National Drought Plan.
+A drought monitoring program identifies climate and water supply trends and detects the emergence or probability of occurrence of droughts, usually by categorizing severity through a percentile ranking approach, and the likely impacts associated with each category. The information can be used to communicate broadly to the general public, as well as to inform specific regional, local, and sector-specific drought management plans and actions. This information can be used to trigger drought mitigation and response measures, as well as disaster declarations and eligibility for drought-related programs, such as disaster relief, insurance, and eligibility for low-interest loans. It can also be used to help inform food relief efforts, water tanker truck deliveries, and other policy and management responses. </t>
+  </si>
+  <si>
     <t xml:space="preserve"> WRM Drought Response</t>
   </si>
   <si>
+    <t xml:space="preserve">During droughts, water use needs to be coordinated at the basin level to ensure water allocations are in alignment with the overall basin drought contingency plan. As highlighted in Chapter 9, the WRM agency should ideally administer a water use permit system that has clear rules of priority during periods of water shortage or drought. Ideally, this permit system would be flexible enough to accommodate priority and equitable use of water during droughts, either through administrative decisions by the WRM agency—preferably within the context of deliberations within the Drought Committee—or through a water rights trading system. The role of conjunctive groundwater management was also highlighted in Chapter 9, underscoring the need to facilitate the storage of water in aquifers during non-drought periods and then abstracting groundwater for use during droughts. The challenge is to ensure that the sustainable yield of an aquifer is not exceeded over the long run.
+The WRM agency often, but not always, serves as the anchor agency for the Drought Committee. In regions where cities, industries, and farms rely heavily on surface water or groundwater, particularly when delivered through regional water conveyance systems, the WRM agency has a critical role to play in drought response. As a core member of the Drought Committee, it should monitor and report on the implementation of the various drought management measures, as well as the overall water balance at the river basin level. The WRM agency also has a central role to play in drought communication and public outreach during droughts, reaching out through its various channels to create a culture of water conservation and water use efficiency. The WRM agency can build upon emergency water conservation activities during droughts to help promote the necessary policy, legal, and institutional reforms to further the agenda of water stewardship. </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Agriculture Drought Response</t>
   </si>
   <si>
+    <t xml:space="preserve">Agriculture, including both crop and livestock production, is an inherently risky endeavor and subject to many types of natural hazards, such as droughts, floods, pestilence, fires, tornadoes, and hail. Agriculture is also confronted with many market risks, such as price fluctuations, logistical interruptions, and sudden export restrictions. Therefore, it is important that the agriculture agency develop a sector-wide agriculture risk management program that considers all risks in a holistic manner to help farmer and livestock producers cope with this broad range of uncertainties (World Bank 2016).
+As highlighted in Chapter 6, climate-smart agriculture programs can help mitigate potential drought impacts by promoting improved agronomic practices. When a severe drought does strike, however, agricultural disaster support programs can be powerful tools to protect the livelihoods of agriculturalists. Such programs can also help de-risk the agricultural sector and contribute to increasing agricultural output through improved access to credit and encouraging agricultural investments. 
+Agricultural disaster support is generally organized around two approaches: (1) direct government-administered relief; and (2) relief administered through agricultural insurance. Direct relief programs provide financial support, such as payments or concessional loans, to agriculturalists who suffer damages due to natural hazards. Natural hazard insurance programs, on the other hand, are typically established, regulated, and subsidized through the agriculture agency, which works through insurance companies that offer plans to agriculturalists. Specialized direct relief or insurance programs are required to deal with different types of producers, for example different programs may be required for annual crops, perennial crops such as orchards or plantations, and livestock. 
+Depending on the specific country context, there may be a mix of direct relief programs and insurance programs. </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Social Protection Drought Response</t>
   </si>
   <si>
+    <t xml:space="preserve">Dedicated agricultural disaster support programs may function well in middle-income countries where the agriculture sector is commercialized, and where agriculturalists have the capacity to apply for assistance. In many developing countries, however, farming and livestock production is managed in a more informal and often subsistence level, and different approaches focused on social protection are required to help rural households respond and recover from droughts (and from floods, for which social protection programs are discussed in Chapter 12). Even with commercialized agriculture, agricultural disaster support programs may not be enough to meet the needs of the impacted population. For example, people employed on farms or who operate as sharecroppers may lose their jobs due to droughts. In addition to their economic impacts, droughts in rural communities may also have deep and long-lasting social impacts related to malnutrition and lack of access to water and sanitation. They can have a profound short-term impact on health as well as longer term impacts such as childhood stunting or lack of access to schooling.
+For these reasons, countries should have preconceived programs for ensuring food and water security in rural areas impacted by natural disasters. Social protection programs that help facilitate effective drought responses in rural areas include offering traditional safety nets and, in extreme conditions, humanitarian aid. </t>
+  </si>
+  <si>
     <t>Flood Monitoring</t>
   </si>
   <si>
+    <t>Flood monitoring, forecasting, and warning is a complex multi-agency process that requires coordination and technical expertise. Figure 12.3 depicts the general relationship between the three key agencies for producing river and coastal flood forecasts and warnings.
+The “weather enterprise” as discussed in Chapter 5, consisting of the NMS working in collaboration with the private sector and regional and global weather centers, is the source of information for weather data and forecasts. This weather information is an essential input into flood forecasts. 
+For coastal flooding, the NMS typically combines weather forecasts and oceanographic information (including tides) with storm surge models to issue forecasts in the form of the storm tide height over normal sea level. Ideally, the coastal floodplains should be mapped, and the forecast can also provide information on how far inland the storm tide will extend and its potential impacts.
+For river flooding, the weather information needs to be combined with watershed hydrological and river hydraulic models to forecast river levels. Ideally, the floodplain will have been mapped and the forecast can include information on the extent and depth of the flooding, as well as potential impacts. Machine-based learning models that correlate weather and watershed conditions to river levels are also becoming more common as a supplement to traditional river flood forecasting methods (Noymanee and Theeramunkong 2019).</t>
+  </si>
+  <si>
     <t>Flood Emergency Preparedness, Response, and Relief</t>
   </si>
   <si>
+    <t>Emergency preparedness and response for floods should take place at many levels: national, regional, local, private sector, and households. The National DRM Plan should include a specific component on disaster response that establishes a standard Emergency Management System (EMS) that allows for multi-agency and multi-jurisdictional responses to emergencies. Some key elements include (1) definition of command structure; (2) regional EOCs; (3) emergency warning dissemination system; (4) master civil defense mutual aid agreements; and (5) multi-agency coordination processes. 
+Although this system is set up to manage all types of emergencies, such as earthquakes, fires, storms, and floods, there also needs to be flood-specific emergency preparedness plans and response actions. The EMS serves to coordinate the actions of the key actors, including relevant national agencies and local governments, and emergency responders such as police, fire, and the military as necessary. The EMS should include provisions as necessary for mobilizing the national level Disaster Management Committee which often consists of Cabinet-level officials and may be chaired by the Executive. 
+For river flooding, the WRM agency should prepare a River Basin Flood Contingency Plan as discussed in Chapter 6, which looks at different flood scenarios and operational responses. The WRM agency should also have a Flood Control Center which serves as the focal point for flood monitoring, forecasting, and operations, working in close collaboration with the DRM agency. In partnership with the DRM agency, the WRM agency also has an important role to play in flood preparedness. Raising awareness about flood risk and emergency response with local governments, businesses, and the private sector is an important preparedness activity. The WRM agency can also provide flood fighting training for its staff, other agencies, and local governments. Finally, the WRM agency should periodically coordinate with the DRM agency and local governments to prepare for local flood and emergency risk management and response.
+Local governments are generally the first responders in a flood emergency, with national assets being deployed as needed—and sometimes with delay. Paralleling the process at the national level, local governments should have Multi-Hazard Mitigation Plans as discussed in Chapter 10 that include floods and should also have Local Emergency Response Plans. To the extent that either river or coastal storms and floods are an issue for the local government, there may be specific Flood Emergency Plans. The local Emergency and Flood Response Plans typically include elements such as: (1) the emergency management organization structure; (2) policies, responsibilities, and procedures to respond to floods; and (3) approaches for after-flood analyses and follow-on activities. Floodplain mapping provides critical information on the potential extent and impacts of floods which can help inform the Emergency Response Plan and flood response actions.</t>
+  </si>
+  <si>
     <t>Flood Disaster Recovery</t>
   </si>
   <si>
+    <t xml:space="preserve">The PDNA should help identify flood impacts and scope out the recovery process, including needs for: (1) housing; (2) restoring public infrastructure and public facilities; (3) restoring business and other organizational assets; and (4) restoring livelihoods. As highlighted in the previous section on flood relief, the PDNA should also identify initiatives to assist impacted people while they are waiting for recovery support. 
+Disaster recovery programs should have dedicated components to meet different needs. For households, support can be provided to repair, replace, or relocate housing. For local governments, support can be provided for emergency works, such as debris removal or flood protection measures, or more permanent works such as roads, water infrastructure, public buildings, and other public utilities. Recovery support can also be provided to businesses and other organizations such as centers of worship or community centers. Finally, recovery support can be provided for flood hazard mitigation projects such as new structural or nature-based projects. 
+Disaster recovery support can be provided in the form of grants, concessional loans, or through subsidized insurance programs. Typically, eligibility for disaster recovery support (except for insurance) is contingent upon a Disaster Declaration, often issued by the Executive. 
+It is important to note that these disaster recovery programs, usually administered or overseen by the DRM agency, can be employed to address a wide variety of potential disasters, for example storms, earthquakes, and fires, as well as floods. However, since the core principle in any disaster recovery effort is to “build back better”, it is important that the programs be tailored to help mitigate the hazard that caused the disaster. For example, if an earthquake resulted in significant destruction of buildings, the DRM agency should ensure adequate buildings regulations in terms of seismic design and require that the buildings regulations are utilized in the reconstruction process. 
+For floods, the disaster recovery programs should consider the principles of floodplain management outlined in Chapter 10 and centered on the PARA concept: protect, avoid, retreat, or accommodate. If these principles are not employed, then the government is potentially creating a moral hazard: people and businesses may not take preventative steps to reduce flood risks on the expectation that future losses will be reimbursed through disaster recovery programs. </t>
+  </si>
+  <si>
     <t>Disaster Risk Financing</t>
   </si>
   <si>
     <t>Disaster Risk Financing Instruments</t>
   </si>
   <si>
+    <t xml:space="preserve">Extreme hydro-climatic events can cause significant financial and economic shocks to households, the private sector, and government budgets. Floods and droughts therefore form a contingent liability for governments since they cause unexpected expenditures and loss of fiscal revenues. Having access to adequate and timely financial resources for response and recovery reduces the impact of these shocks and helps the economy bounce back quickly. A lack of such resources causes a delay in the provision of life-saving responses and pushes back the reconstruction of critical public and private structures, facilities, and infrastructure, which brings higher long-term impacts of a disaster and a more significant effect on poverty and development.
+There are a variety of risk financing instruments, each with specific characteristics that make each type well-suited to address certain situations but less effective in others. The optimal mix of instruments depends on the overall fiscal situation of the country as well as its disaster risk profile. </t>
+  </si>
+  <si>
     <t>Disaster Risk Financing National Sector Framework</t>
+  </si>
+  <si>
+    <t>Two sets of laws provide the foundation for the legal and regulatory framework for disaster risk finance: budgetary laws and DRM laws. The budgetary law should explicitly authorize the finance agency to develop and implement a disaster risk financing strategy. Another important element concerns the process by which the is budget allocated, and level of discretionary funding by national agencies or local governments to accommodate the needs during the response, relief, and recovery phases. The budget law should also include a provision for a national disaster fund, including guidelines for the size of the fund, and its utilization. Of importance are the emergency procurement procedures that may need to be employed to rapidly respond to disaster needs.
+The DRM law should mandate the DRM agency to work with the finance agency to develop a disaster risk financing strategy. The role of the DRM agency in administering or overseeing disaster funds should be outlined in the DRM or budget law. The law should require the DRM agency to develop procedures for recommending or declaring a state of national emergency, as this may be used to trigger contingent credit lines or provide access to a national disaster fund.</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1076,7 +1262,7 @@
     <col min="4" max="4" width="82.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1086,364 +1272,610 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>95</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>97</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>100</v>
+      </c>
+      <c r="C43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>102</v>
+      </c>
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: Updated key agency actions questions xlsx and related test
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/keyagencyactionsquestions.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/keyagencyactionsquestions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B5321F-93A1-407F-9BCE-A0DC67505E74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D49A478-2CBF-44C5-AD3A-C029175BA41D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keyagencyactionsquestions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="253">
   <si>
     <t xml:space="preserve"> Question</t>
   </si>
@@ -919,6 +919,9 @@
   </si>
   <si>
     <t>Is there a collaboration between the NMS/NHS and the WRM Agency in cases where the WRM agency is responsible for flood forecasts so the NMS/NHS draws from the weather enterprise the information required by the WRM to deliver river flood forecasts as well as coastal storms for river coastal interactions? Is this collaboration facilitated through an inter agency agreement or through a Flood Forecasting Center?</t>
+  </si>
+  <si>
+    <t>Do the WRM, DRM and drought national strategic plans provide a platform to advocate for sustainable funding for hydro-met services?</t>
   </si>
 </sst>
 </file>
@@ -1775,17 +1778,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2124,7 +2128,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2134,8 +2138,8 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="D25" t="s">
-        <v>179</v>
+      <c r="D25" s="4" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2149,32 +2153,32 @@
         <v>47</v>
       </c>
       <c r="D26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" t="s">
-        <v>140</v>
-      </c>
-      <c r="D27" t="s">
-        <v>139</v>
-      </c>
-    </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
       <c r="B28" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>113</v>
+      <c r="C28" t="s">
+        <v>140</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2185,13 +2189,13 @@
         <v>106</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2199,13 +2203,13 @@
         <v>106</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2213,10 +2217,10 @@
         <v>106</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" t="s">
-        <v>183</v>
+        <v>108</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,24 +2231,24 @@
         <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>141</v>
+        <v>106</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2258,7 +2262,7 @@
         <v>146</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2272,7 +2276,7 @@
         <v>146</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2286,7 +2290,7 @@
         <v>146</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2300,7 +2304,7 @@
         <v>146</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,7 +2318,7 @@
         <v>146</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,21 +2332,21 @@
         <v>146</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>187</v>
+        <v>146</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2356,10 +2360,10 @@
         <v>147</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2370,10 +2374,10 @@
         <v>147</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -2383,8 +2387,8 @@
       <c r="C43" t="s">
         <v>147</v>
       </c>
-      <c r="D43" t="s">
-        <v>190</v>
+      <c r="D43" s="4" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2397,8 +2401,8 @@
       <c r="C44" t="s">
         <v>147</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>191</v>
+      <c r="D44" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2412,7 +2416,7 @@
         <v>147</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2426,7 +2430,7 @@
         <v>147</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2434,13 +2438,13 @@
         <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D47" t="s">
-        <v>50</v>
+        <v>147</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2454,7 +2458,7 @@
         <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2468,7 +2472,7 @@
         <v>148</v>
       </c>
       <c r="D49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2482,7 +2486,7 @@
         <v>148</v>
       </c>
       <c r="D50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,7 +2500,7 @@
         <v>148</v>
       </c>
       <c r="D51" t="s">
-        <v>194</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,13 +2508,13 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2524,7 +2528,7 @@
         <v>149</v>
       </c>
       <c r="D53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2538,7 +2542,7 @@
         <v>149</v>
       </c>
       <c r="D54" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2552,7 +2556,7 @@
         <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2566,21 +2570,21 @@
         <v>149</v>
       </c>
       <c r="D56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>150</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>200</v>
+        <v>149</v>
+      </c>
+      <c r="D57" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2594,7 +2598,7 @@
         <v>150</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2608,7 +2612,7 @@
         <v>150</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2622,7 +2626,7 @@
         <v>150</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2636,7 +2640,7 @@
         <v>150</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2650,24 +2654,24 @@
         <v>150</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2678,10 +2682,10 @@
         <v>151</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -2692,7 +2696,7 @@
         <v>151</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2706,10 +2710,10 @@
         <v>151</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>20</v>
       </c>
@@ -2720,10 +2724,10 @@
         <v>151</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -2734,21 +2738,21 @@
         <v>151</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>152</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>54</v>
+        <v>151</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2762,7 +2766,7 @@
         <v>152</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2776,7 +2780,7 @@
         <v>152</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2790,7 +2794,7 @@
         <v>152</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>213</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2804,7 +2808,7 @@
         <v>152</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>56</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2818,7 +2822,7 @@
         <v>152</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2832,7 +2836,7 @@
         <v>152</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>214</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2840,13 +2844,13 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>169</v>
+        <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2860,7 +2864,7 @@
         <v>48</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>58</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2874,7 +2878,7 @@
         <v>48</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2888,7 +2892,7 @@
         <v>48</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>218</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2899,10 +2903,10 @@
         <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2916,7 +2920,7 @@
         <v>49</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2930,7 +2934,7 @@
         <v>49</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2944,21 +2948,21 @@
         <v>49</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>153</v>
+        <v>169</v>
+      </c>
+      <c r="C84" t="s">
+        <v>49</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2972,7 +2976,7 @@
         <v>153</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2986,38 +2990,38 @@
         <v>153</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
       <c r="B87" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>22</v>
       </c>
       <c r="B88" t="s">
         <v>24</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="2" t="s">
         <v>154</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -3028,7 +3032,7 @@
         <v>154</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3042,7 +3046,7 @@
         <v>154</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3056,7 +3060,7 @@
         <v>154</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3070,10 +3074,10 @@
         <v>154</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>22</v>
       </c>
@@ -3084,35 +3088,35 @@
         <v>154</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>22</v>
       </c>
       <c r="B94" t="s">
         <v>24</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" t="s">
         <v>154</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>22</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C95" t="s">
-        <v>155</v>
-      </c>
-      <c r="D95" t="s">
-        <v>60</v>
+        <v>24</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3126,7 +3130,7 @@
         <v>155</v>
       </c>
       <c r="D96" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3140,7 +3144,7 @@
         <v>155</v>
       </c>
       <c r="D97" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3154,7 +3158,7 @@
         <v>155</v>
       </c>
       <c r="D98" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3168,7 +3172,7 @@
         <v>155</v>
       </c>
       <c r="D99" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3182,7 +3186,7 @@
         <v>155</v>
       </c>
       <c r="D100" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3196,7 +3200,7 @@
         <v>155</v>
       </c>
       <c r="D101" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3210,21 +3214,21 @@
         <v>155</v>
       </c>
       <c r="D102" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B103" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C103" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D103" t="s">
-        <v>232</v>
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3238,7 +3242,7 @@
         <v>156</v>
       </c>
       <c r="D104" t="s">
-        <v>68</v>
+        <v>232</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3252,7 +3256,7 @@
         <v>156</v>
       </c>
       <c r="D105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,7 +3270,7 @@
         <v>156</v>
       </c>
       <c r="D106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3280,7 +3284,7 @@
         <v>156</v>
       </c>
       <c r="D107" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3288,13 +3292,13 @@
         <v>26</v>
       </c>
       <c r="B108" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C108" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D108" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3308,7 +3312,7 @@
         <v>157</v>
       </c>
       <c r="D109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3322,7 +3326,7 @@
         <v>157</v>
       </c>
       <c r="D110" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3336,7 +3340,7 @@
         <v>157</v>
       </c>
       <c r="D111" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3350,21 +3354,21 @@
         <v>157</v>
       </c>
       <c r="D112" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B113" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C113" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D113" t="s">
-        <v>233</v>
+        <v>76</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3378,7 +3382,7 @@
         <v>158</v>
       </c>
       <c r="D114" t="s">
-        <v>77</v>
+        <v>233</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3392,7 +3396,7 @@
         <v>158</v>
       </c>
       <c r="D115" t="s">
-        <v>234</v>
+        <v>77</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3406,7 +3410,7 @@
         <v>158</v>
       </c>
       <c r="D116" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3420,7 +3424,7 @@
         <v>158</v>
       </c>
       <c r="D117" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3428,13 +3432,13 @@
         <v>29</v>
       </c>
       <c r="B118" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C118" t="s">
-        <v>159</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>237</v>
+        <v>158</v>
+      </c>
+      <c r="D118" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3448,7 +3452,7 @@
         <v>159</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3462,7 +3466,7 @@
         <v>159</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3476,7 +3480,7 @@
         <v>159</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,13 +3488,13 @@
         <v>29</v>
       </c>
       <c r="B122" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C122" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,7 +3508,7 @@
         <v>160</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3518,7 +3522,7 @@
         <v>160</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3532,21 +3536,21 @@
         <v>160</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>243</v>
+        <v>78</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>170</v>
+        <v>29</v>
       </c>
       <c r="B126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>79</v>
+        <v>243</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3560,7 +3564,7 @@
         <v>161</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,7 +3578,7 @@
         <v>161</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3588,7 +3592,7 @@
         <v>161</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,13 +3600,13 @@
         <v>170</v>
       </c>
       <c r="B130" t="s">
-        <v>34</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>162</v>
+        <v>33</v>
+      </c>
+      <c r="C130" t="s">
+        <v>161</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>244</v>
+        <v>82</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3616,7 +3620,7 @@
         <v>162</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,7 +3634,7 @@
         <v>162</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3638,13 +3642,13 @@
         <v>170</v>
       </c>
       <c r="B133" t="s">
-        <v>35</v>
-      </c>
-      <c r="C133" t="s">
-        <v>163</v>
+        <v>34</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>83</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,7 +3662,7 @@
         <v>163</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>247</v>
+        <v>83</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3672,7 +3676,7 @@
         <v>163</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3686,7 +3690,7 @@
         <v>163</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3694,13 +3698,13 @@
         <v>170</v>
       </c>
       <c r="B137" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C137" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>84</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3714,7 +3718,7 @@
         <v>164</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3728,21 +3732,21 @@
         <v>164</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>170</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" t="s">
         <v>36</v>
       </c>
       <c r="C140" t="s">
         <v>164</v>
       </c>
-      <c r="D140" s="6" t="s">
-        <v>87</v>
+      <c r="D140" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3756,24 +3760,24 @@
         <v>164</v>
       </c>
       <c r="D141" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>170</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C142" t="s">
+        <v>164</v>
+      </c>
+      <c r="D142" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C142" t="s">
-        <v>165</v>
-      </c>
-      <c r="D142" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>171</v>
       </c>
@@ -3783,8 +3787,8 @@
       <c r="C143" t="s">
         <v>165</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>251</v>
+      <c r="D143" s="5" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,7 +3802,7 @@
         <v>165</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>89</v>
+        <v>251</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,7 +3816,7 @@
         <v>165</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3820,13 +3824,13 @@
         <v>171</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="C146" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3840,7 +3844,7 @@
         <v>166</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3854,7 +3858,7 @@
         <v>166</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3868,7 +3872,7 @@
         <v>166</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3882,7 +3886,7 @@
         <v>166</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3896,7 +3900,7 @@
         <v>166</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3910,7 +3914,7 @@
         <v>166</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3924,7 +3928,7 @@
         <v>166</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3932,13 +3936,13 @@
         <v>171</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C154" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3952,7 +3956,7 @@
         <v>167</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3966,21 +3970,21 @@
         <v>167</v>
       </c>
       <c r="D156" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C157" t="s">
+        <v>167</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C157" t="s">
-        <v>168</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3994,7 +3998,7 @@
         <v>168</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4008,7 +4012,7 @@
         <v>168</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4022,13 +4026,27 @@
         <v>168</v>
       </c>
       <c r="D160" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C161" t="s">
+        <v>168</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
-      <c r="D161" s="1"/>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="D162" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4037,6 +4055,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CF95EF2F384F0419312B394CBDE3AE2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6efdc87a01d4ba6154ecd9afe69b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="18fba281-3140-4e33-b78f-87df0c1efb23" xmlns:ns4="f7620e32-1325-4c29-861c-5840d24c4310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef933d5bbd2bd3eb58c8ad997b164a29" ns3:_="" ns4:_="">
     <xsd:import namespace="18fba281-3140-4e33-b78f-87df0c1efb23"/>
@@ -4265,22 +4298,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56B50B3F-65EA-4DF6-B2B2-B86F192854FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15D48028-CB17-47FE-8640-1B6F042B0343}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6A13AE-37E0-4EFF-97D8-0C2932CFB4EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4297,29 +4340,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56B50B3F-65EA-4DF6-B2B2-B86F192854FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15D48028-CB17-47FE-8640-1B6F042B0343}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>